<commit_message>
apparently its not actually that heavy
</commit_message>
<xml_diff>
--- a/changes/ak-stocks.xlsx
+++ b/changes/ak-stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1035AB-B87A-499F-81E4-DAABE704A3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97410066-1465-4E5E-B2D9-741965459BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1338,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U57" sqref="U57"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,7 +1418,7 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>0.3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E3">
         <v>-8</v>
@@ -1431,10 +1431,10 @@
       </c>
       <c r="N3">
         <f>C3-D3*20-E3*0.8-F3*0.6-I3*5</f>
-        <v>23.2</v>
+        <v>23.4</v>
       </c>
       <c r="P3">
-        <v>15.8733</v>
+        <v>14.356517999999999</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>15</v>
       </c>
       <c r="D4">
-        <v>0.3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E4">
         <v>-8</v>
@@ -1461,10 +1461,10 @@
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N50" si="0">C4-D4*20-E4*0.8-F4*0.6-I4*5</f>
-        <v>23.2</v>
+        <v>23.4</v>
       </c>
       <c r="P4">
-        <v>15.8733</v>
+        <v>14.356517999999999</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1478,23 +1478,23 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="E5">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="F5">
-        <v>-13</v>
+        <v>-11</v>
       </c>
       <c r="M5">
         <v>600</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>23.400000000000002</v>
+        <v>23.6</v>
       </c>
       <c r="P5">
-        <v>12.3459</v>
+        <v>10.987850999999999</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1508,23 +1508,23 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="E6">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="F6">
-        <v>-13</v>
+        <v>-11</v>
       </c>
       <c r="M6">
         <v>600</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>23.400000000000002</v>
+        <v>23.6</v>
       </c>
       <c r="P6">
-        <v>12.3459</v>
+        <v>10.987850999999999</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="D53">
         <f t="shared" si="1"/>
-        <v>0.35</v>
+        <v>0.33999999999999997</v>
       </c>
       <c r="E53">
         <f t="shared" si="1"/>
@@ -2713,7 +2713,7 @@
       </c>
       <c r="N53">
         <f t="shared" si="1"/>
-        <v>22.2</v>
+        <v>22.4</v>
       </c>
       <c r="O53">
         <f t="shared" si="1"/>
@@ -2721,11 +2721,11 @@
       </c>
       <c r="P53">
         <f t="shared" si="1"/>
-        <v>15.8733</v>
+        <v>14.356517999999999</v>
       </c>
       <c r="Q53">
         <f>P53*0.024</f>
-        <v>0.3809592</v>
+        <v>0.34455643199999997</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
@@ -2739,15 +2739,15 @@
       </c>
       <c r="D54">
         <f t="shared" si="2"/>
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
       <c r="E54">
         <f t="shared" si="2"/>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="F54">
         <f t="shared" si="2"/>
-        <v>-13</v>
+        <v>-11</v>
       </c>
       <c r="G54">
         <f t="shared" si="2"/>
@@ -2779,7 +2779,7 @@
       </c>
       <c r="N54">
         <f t="shared" si="2"/>
-        <v>22.400000000000002</v>
+        <v>22.6</v>
       </c>
       <c r="O54">
         <f t="shared" si="2"/>
@@ -2787,11 +2787,11 @@
       </c>
       <c r="P54">
         <f t="shared" si="2"/>
-        <v>12.3459</v>
+        <v>10.987850999999999</v>
       </c>
       <c r="Q54">
         <f t="shared" ref="Q54:Q89" si="3">P54*0.024</f>
-        <v>0.2963016</v>
+        <v>0.263708424</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
@@ -2800,12 +2800,12 @@
         <v>114</v>
       </c>
       <c r="C55">
-        <f t="shared" ref="C55:P55" si="4">C53+C9</f>
+        <f>C4+C7+C9</f>
         <v>16</v>
       </c>
       <c r="D55">
-        <f t="shared" si="4"/>
-        <v>0.43999999999999995</v>
+        <f t="shared" ref="D55:P55" si="4">D4+D7+D9</f>
+        <v>0.42999999999999994</v>
       </c>
       <c r="E55">
         <f t="shared" si="4"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="N55">
         <f t="shared" si="4"/>
-        <v>22.8</v>
+        <v>23</v>
       </c>
       <c r="O55">
         <f t="shared" si="4"/>
@@ -2853,11 +2853,11 @@
       </c>
       <c r="P55">
         <f t="shared" si="4"/>
-        <v>21.8733</v>
+        <v>20.356518000000001</v>
       </c>
       <c r="Q55">
         <f t="shared" si="3"/>
-        <v>0.52495920000000007</v>
+        <v>0.48855643200000004</v>
       </c>
       <c r="S55" t="s">
         <v>75</v>
@@ -2869,20 +2869,20 @@
         <v>115</v>
       </c>
       <c r="C56">
-        <f t="shared" ref="C56:M56" si="5">C54+C9</f>
+        <f>C5+C7+C9</f>
         <v>16</v>
       </c>
       <c r="D56">
-        <f t="shared" si="5"/>
-        <v>0.39</v>
+        <f t="shared" ref="D56:P56" si="5">D5+D7+D9</f>
+        <v>0.36</v>
       </c>
       <c r="E56">
         <f t="shared" si="5"/>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="F56">
         <f t="shared" si="5"/>
-        <v>-14</v>
+        <v>-12</v>
       </c>
       <c r="G56">
         <f t="shared" si="5"/>
@@ -2913,16 +2913,20 @@
         <v>1200</v>
       </c>
       <c r="N56">
-        <f>SUM(N4,N9)</f>
-        <v>23.8</v>
+        <f t="shared" si="5"/>
+        <v>23.200000000000003</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="P56">
-        <f>SUM(P4,P9)</f>
-        <v>21.8733</v>
+        <f t="shared" si="5"/>
+        <v>16.987850999999999</v>
       </c>
       <c r="Q56">
         <f t="shared" si="3"/>
-        <v>0.52495920000000007</v>
+        <v>0.40770842400000001</v>
       </c>
       <c r="S56" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
ak stock fix + hera stock fix
</commit_message>
<xml_diff>
--- a/changes/ak-stocks.xlsx
+++ b/changes/ak-stocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97410066-1465-4E5E-B2D9-741965459BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B50D3B6-BB4D-4CC1-B27A-29A858591053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="128">
   <si>
     <t>CURRENT</t>
   </si>
@@ -384,6 +384,42 @@
   </si>
   <si>
     <t>Izhmash AK-74 Polymer 6P20 Sb.7 + pad</t>
+  </si>
+  <si>
+    <t>ak12_gen2_stock</t>
+  </si>
+  <si>
+    <t>Kalashnikov Concern AK-12 Gen 2</t>
+  </si>
+  <si>
+    <t>kalashnikov_concern_rpl_20_stock</t>
+  </si>
+  <si>
+    <t>Kalashnikov Concern RPL-20 Stock</t>
+  </si>
+  <si>
+    <t>kalashnikov_concern_ak12_gen3_stock_cheekpad</t>
+  </si>
+  <si>
+    <t>Kalashnikov Concern AK-12 Gen 3 Stock Cheekpad</t>
+  </si>
+  <si>
+    <t>kalashnikov_concern_ak12_gen3_stock_cheekpad_extended</t>
+  </si>
+  <si>
+    <t>Kalashnikov Concern AK-12 Gen 3 Stock Cheekpad Extended</t>
+  </si>
+  <si>
+    <t>rpl_20_cheek_pad_high</t>
+  </si>
+  <si>
+    <t>RPL-20 Cheek Pad High</t>
+  </si>
+  <si>
+    <t>rpl_20_cheek_pad_low</t>
+  </si>
+  <si>
+    <t>RPL-20 Cheek Pad Low</t>
   </si>
 </sst>
 </file>
@@ -532,7 +568,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="48">
+  <fills count="49">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -802,6 +838,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -963,7 +1005,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -981,6 +1023,8 @@
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1336,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S89"/>
+  <dimension ref="A1:S106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S44" sqref="S44"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N50" si="0">C4-D4*20-E4*0.8-F4*0.6-I4*5</f>
+        <f t="shared" ref="N4:N56" si="0">C4-D4*20-E4*0.8-F4*0.6-I4*5</f>
         <v>23.4</v>
       </c>
       <c r="P4">
@@ -2198,23 +2242,20 @@
         <v>-1</v>
       </c>
       <c r="D34">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>-0.1</v>
+        <v>-1</v>
       </c>
       <c r="M34">
         <v>500</v>
       </c>
       <c r="N34">
         <f t="shared" si="0"/>
-        <v>-2.5</v>
+        <v>-2.6</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -2429,7 +2470,7 @@
         <v>10</v>
       </c>
       <c r="D42">
-        <v>0.35</v>
+        <v>0.42</v>
       </c>
       <c r="E42">
         <v>-15</v>
@@ -2442,1651 +2483,2345 @@
       </c>
       <c r="N42">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>25.6</v>
+      </c>
+      <c r="P42">
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E43">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="F43">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="M43">
         <v>0</v>
       </c>
       <c r="N43">
         <f t="shared" si="0"/>
-        <v>3.8</v>
+        <v>1.8000000000000003</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D44">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="M44">
         <v>250</v>
       </c>
       <c r="N44">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C45">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D45">
-        <v>0.1</v>
-      </c>
-      <c r="E45">
-        <v>-1</v>
+        <v>0.06</v>
       </c>
       <c r="M45">
         <v>500</v>
       </c>
       <c r="N45">
         <f t="shared" si="0"/>
-        <v>2.8</v>
+        <v>-0.19999999999999996</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C46">
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="D46">
-        <v>0.15</v>
-      </c>
-      <c r="E46">
-        <v>-2</v>
-      </c>
-      <c r="F46">
-        <v>-1</v>
+        <v>0.09</v>
       </c>
       <c r="M46">
         <v>750</v>
       </c>
       <c r="N46">
         <f t="shared" si="0"/>
-        <v>5.1999999999999993</v>
+        <v>-0.29999999999999982</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47">
+        <v>16</v>
+      </c>
+      <c r="D47">
+        <v>0.2</v>
+      </c>
+      <c r="E47">
+        <v>-11</v>
+      </c>
+      <c r="F47">
+        <v>-6</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="0"/>
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>0.06</v>
+      </c>
+      <c r="M48">
+        <v>600</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49">
+        <v>0.06</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="M49">
+        <v>600</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="0"/>
+        <v>0.79999999999999982</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <v>0.24</v>
+      </c>
+      <c r="E50">
+        <v>-14</v>
+      </c>
+      <c r="F50">
+        <v>-17</v>
+      </c>
+      <c r="H50">
+        <v>0.05</v>
+      </c>
+      <c r="M50">
+        <v>2000</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="0"/>
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>0.08</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999991</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <v>0.08</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <f>C52-D52*20-E52*0.8-F52*0.6-I52*5</f>
+        <v>0.39999999999999991</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B53" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
         <v>0.1</v>
       </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="M47">
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="M53">
         <v>1200</v>
       </c>
-      <c r="N47">
+      <c r="N53">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="P47">
+      <c r="P53">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B54" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
         <v>0.13</v>
       </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="M48">
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="M54">
         <v>400</v>
       </c>
-      <c r="N48">
+      <c r="N54">
         <f t="shared" si="0"/>
         <v>-2.6</v>
       </c>
-      <c r="P48">
+      <c r="P54">
         <v>9.35</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
-      <c r="B49" s="12" t="s">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" s="11"/>
+      <c r="B55" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C49">
+      <c r="C55">
         <v>18</v>
       </c>
-      <c r="D49">
+      <c r="D55">
         <v>0.21</v>
       </c>
-      <c r="E49">
+      <c r="E55">
         <v>-10</v>
       </c>
-      <c r="F49">
+      <c r="F55">
         <v>-9</v>
       </c>
-      <c r="M49">
+      <c r="M55">
         <v>800</v>
       </c>
-      <c r="N49">
+      <c r="N55">
         <f t="shared" si="0"/>
         <v>27.2</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="12" t="s">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="B56" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C50">
+      <c r="C56">
         <v>17</v>
       </c>
-      <c r="D50">
+      <c r="D56">
         <v>0.34</v>
       </c>
-      <c r="E50">
+      <c r="E56">
         <v>-11</v>
       </c>
-      <c r="F50">
+      <c r="F56">
         <v>-10</v>
       </c>
-      <c r="M50">
+      <c r="M56">
         <v>1400</v>
       </c>
-      <c r="N50">
+      <c r="N56">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="P50">
+      <c r="P56">
         <v>15.4</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A53" s="9"/>
-      <c r="B53" s="9" t="s">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A59" s="9"/>
+      <c r="B59" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C53">
-        <f t="shared" ref="C53:P53" si="1">C4+C7</f>
+      <c r="C59">
+        <f>C4+C7</f>
         <v>15</v>
       </c>
-      <c r="D53">
-        <f t="shared" si="1"/>
+      <c r="D59">
+        <f>D4+D7</f>
         <v>0.33999999999999997</v>
       </c>
-      <c r="E53">
-        <f t="shared" si="1"/>
+      <c r="E59">
+        <f>E4+E7</f>
         <v>-8</v>
       </c>
-      <c r="F53">
-        <f t="shared" si="1"/>
+      <c r="F59">
+        <f>F4+F7</f>
         <v>-13</v>
       </c>
-      <c r="G53">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I53">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J53">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K53">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L53">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M53">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N53">
-        <f t="shared" si="1"/>
+      <c r="G59">
+        <f>G4+G7</f>
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <f>H4+H7</f>
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <f>I4+I7</f>
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <f>J4+J7</f>
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <f>K4+K7</f>
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <f>L4+L7</f>
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <f>M4+M7</f>
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <f>N4+N7</f>
         <v>22.4</v>
       </c>
-      <c r="O53">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P53">
-        <f t="shared" si="1"/>
+      <c r="O59">
+        <f>O4+O7</f>
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <f>P4+P7</f>
         <v>14.356517999999999</v>
       </c>
-      <c r="Q53">
-        <f>P53*0.024</f>
+      <c r="Q59">
+        <f>P59*0.024</f>
         <v>0.34455643199999997</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9" t="s">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A60" s="9"/>
+      <c r="B60" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C54">
-        <f t="shared" ref="C54:P54" si="2">C5+C7</f>
+      <c r="C60">
+        <f>C5+C7</f>
         <v>15</v>
       </c>
-      <c r="D54">
-        <f t="shared" si="2"/>
+      <c r="D60">
+        <f>D5+D7</f>
         <v>0.27</v>
       </c>
-      <c r="E54">
-        <f t="shared" si="2"/>
+      <c r="E60">
+        <f>E5+E7</f>
         <v>-8</v>
       </c>
-      <c r="F54">
-        <f t="shared" si="2"/>
+      <c r="F60">
+        <f>F5+F7</f>
         <v>-11</v>
       </c>
-      <c r="G54">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I54">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J54">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K54">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L54">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M54">
-        <f t="shared" si="2"/>
+      <c r="G60">
+        <f>G5+G7</f>
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <f>H5+H7</f>
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <f>I5+I7</f>
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <f>J5+J7</f>
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <f>K5+K7</f>
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <f>L5+L7</f>
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <f>M5+M7</f>
         <v>600</v>
       </c>
-      <c r="N54">
-        <f t="shared" si="2"/>
+      <c r="N60">
+        <f>N5+N7</f>
         <v>22.6</v>
       </c>
-      <c r="O54">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P54">
-        <f t="shared" si="2"/>
+      <c r="O60">
+        <f>O5+O7</f>
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <f>P5+P7</f>
         <v>10.987850999999999</v>
       </c>
-      <c r="Q54">
-        <f t="shared" ref="Q54:Q89" si="3">P54*0.024</f>
+      <c r="Q60">
+        <f t="shared" ref="Q60:Q106" si="1">P60*0.024</f>
         <v>0.263708424</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A55" s="9"/>
-      <c r="B55" s="14" t="s">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A61" s="9"/>
+      <c r="B61" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="C55">
+      <c r="C61">
         <f>C4+C7+C9</f>
         <v>16</v>
       </c>
-      <c r="D55">
-        <f t="shared" ref="D55:P55" si="4">D4+D7+D9</f>
+      <c r="D61">
+        <f>D4+D7+D9</f>
         <v>0.42999999999999994</v>
       </c>
-      <c r="E55">
-        <f t="shared" si="4"/>
+      <c r="E61">
+        <f>E4+E7+E9</f>
         <v>-9</v>
       </c>
-      <c r="F55">
-        <f t="shared" si="4"/>
+      <c r="F61">
+        <f>F4+F7+F9</f>
         <v>-14</v>
       </c>
-      <c r="G55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M55">
-        <f t="shared" si="4"/>
+      <c r="G61">
+        <f>G4+G7+G9</f>
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <f>H4+H7+H9</f>
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <f>I4+I7+I9</f>
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <f>J4+J7+J9</f>
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <f>K4+K7+K9</f>
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <f>L4+L7+L9</f>
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <f>M4+M7+M9</f>
         <v>600</v>
       </c>
-      <c r="N55">
-        <f t="shared" si="4"/>
+      <c r="N61">
+        <f>N4+N7+N9</f>
         <v>23</v>
       </c>
-      <c r="O55">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P55">
-        <f t="shared" si="4"/>
+      <c r="O61">
+        <f>O4+O7+O9</f>
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <f>P4+P7+P9</f>
         <v>20.356518000000001</v>
       </c>
-      <c r="Q55">
-        <f t="shared" si="3"/>
+      <c r="Q61">
+        <f t="shared" si="1"/>
         <v>0.48855643200000004</v>
       </c>
-      <c r="S55" t="s">
+      <c r="S61" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A56" s="9"/>
-      <c r="B56" s="14" t="s">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A62" s="9"/>
+      <c r="B62" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="C56">
+      <c r="C62">
         <f>C5+C7+C9</f>
         <v>16</v>
       </c>
-      <c r="D56">
-        <f t="shared" ref="D56:P56" si="5">D5+D7+D9</f>
+      <c r="D62">
+        <f>D5+D7+D9</f>
         <v>0.36</v>
       </c>
-      <c r="E56">
-        <f t="shared" si="5"/>
+      <c r="E62">
+        <f>E5+E7+E9</f>
         <v>-9</v>
       </c>
-      <c r="F56">
-        <f t="shared" si="5"/>
+      <c r="F62">
+        <f>F5+F7+F9</f>
         <v>-12</v>
       </c>
-      <c r="G56">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J56">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K56">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L56">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M56">
-        <f t="shared" si="5"/>
+      <c r="G62">
+        <f>G5+G7+G9</f>
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <f>H5+H7+H9</f>
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <f>I5+I7+I9</f>
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <f>J5+J7+J9</f>
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <f>K5+K7+K9</f>
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <f>L5+L7+L9</f>
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <f>M5+M7+M9</f>
         <v>1200</v>
       </c>
-      <c r="N56">
-        <f t="shared" si="5"/>
+      <c r="N62">
+        <f>N5+N7+N9</f>
         <v>23.200000000000003</v>
       </c>
-      <c r="O56">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P56">
-        <f t="shared" si="5"/>
+      <c r="O62">
+        <f>O5+O7+O9</f>
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <f>P5+P7+P9</f>
         <v>16.987850999999999</v>
       </c>
-      <c r="Q56">
-        <f t="shared" si="3"/>
+      <c r="Q62">
+        <f t="shared" si="1"/>
         <v>0.40770842400000001</v>
       </c>
-      <c r="S56" t="s">
+      <c r="S62" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q57">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16" t="s">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A64" s="16"/>
+      <c r="B64" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C58">
+      <c r="C64">
         <f>C10</f>
         <v>13</v>
       </c>
-      <c r="D58">
-        <f t="shared" ref="D58:P58" si="6">D10</f>
+      <c r="D64">
+        <f>D10</f>
         <v>0.19</v>
       </c>
-      <c r="E58">
-        <f t="shared" si="6"/>
+      <c r="E64">
+        <f>E10</f>
         <v>-8</v>
       </c>
-      <c r="F58">
-        <f t="shared" si="6"/>
+      <c r="F64">
+        <f>F10</f>
         <v>-11</v>
       </c>
-      <c r="G58">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H58">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I58">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J58">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K58">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L58">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M58">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N58">
-        <f t="shared" si="6"/>
+      <c r="G64">
+        <f>G10</f>
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <f>H10</f>
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <f>I10</f>
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <f>J10</f>
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <f>K10</f>
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <f>L10</f>
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <f>M10</f>
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <f>N10</f>
         <v>22.2</v>
       </c>
-      <c r="O58">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P58">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q58">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S58" t="s">
+      <c r="O64">
+        <f>O10</f>
+        <v>0</v>
+      </c>
+      <c r="P64">
+        <f>P10</f>
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S64" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
-      <c r="B59" s="16" t="s">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A65" s="16"/>
+      <c r="B65" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C59">
+      <c r="C65">
         <f>C11</f>
         <v>14</v>
       </c>
-      <c r="D59">
+      <c r="D65">
         <f>D11</f>
         <v>0.2</v>
       </c>
-      <c r="E59">
+      <c r="E65">
         <v>-7</v>
       </c>
-      <c r="F59">
+      <c r="F65">
         <v>12</v>
       </c>
-      <c r="G59">
-        <f t="shared" ref="G59:P59" si="7">G11</f>
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I59">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J59">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="K59">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L59">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="M59">
-        <f t="shared" si="7"/>
+      <c r="G65">
+        <f>G11</f>
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <f>H11</f>
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <f>I11</f>
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <f>J11</f>
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <f>K11</f>
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <f>L11</f>
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <f>M11</f>
         <v>300</v>
       </c>
-      <c r="N59">
-        <f t="shared" si="7"/>
+      <c r="N65">
+        <f>N11</f>
         <v>22.200000000000003</v>
       </c>
-      <c r="O59">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P59">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q59">
-        <f>P59*0.024</f>
-        <v>0</v>
-      </c>
-      <c r="S59" t="s">
+      <c r="O65">
+        <f>O11</f>
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <f>P11</f>
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S65" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q60">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4" t="s">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q61">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="1" t="s">
+      <c r="Q67">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C62">
+      <c r="C68">
         <f>SUM(C14,C15,C16,C12)</f>
         <v>22</v>
       </c>
-      <c r="D62">
-        <f t="shared" ref="D62:P62" si="8">SUM(D14,D15,D16,D12)</f>
+      <c r="D68">
+        <f>SUM(D14,D15,D16,D12)</f>
         <v>0.43</v>
       </c>
-      <c r="E62">
-        <f t="shared" si="8"/>
+      <c r="E68">
+        <f>SUM(E14,E15,E16,E12)</f>
         <v>-8</v>
       </c>
-      <c r="F62">
-        <f t="shared" si="8"/>
+      <c r="F68">
+        <f>SUM(F14,F15,F16,F12)</f>
         <v>-7</v>
       </c>
-      <c r="G62">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H62">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I62">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="J62">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K62">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L62">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="M62">
-        <f t="shared" si="8"/>
+      <c r="G68">
+        <f>SUM(G14,G15,G16,G12)</f>
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <f>SUM(H14,H15,H16,H12)</f>
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <f>SUM(I14,I15,I16,I12)</f>
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <f>SUM(J14,J15,J16,J12)</f>
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <f>SUM(K14,K15,K16,K12)</f>
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <f>SUM(L14,L15,L16,L12)</f>
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <f>SUM(M14,M15,M16,M12)</f>
         <v>1400</v>
       </c>
-      <c r="N62">
-        <f t="shared" si="8"/>
+      <c r="N68">
+        <f>SUM(N14,N15,N16,N12)</f>
         <v>23.999999999999996</v>
       </c>
-      <c r="O62">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P62">
-        <f t="shared" si="8"/>
+      <c r="O68">
+        <f>SUM(O14,O15,O16,O12)</f>
+        <v>0</v>
+      </c>
+      <c r="P68">
+        <f>SUM(P14,P15,P16,P12)</f>
         <v>19.399999999999999</v>
       </c>
-      <c r="Q62">
-        <f t="shared" si="3"/>
+      <c r="Q68">
+        <f t="shared" si="1"/>
         <v>0.46559999999999996</v>
       </c>
-      <c r="S62" t="s">
+      <c r="S68" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="2" t="s">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C63">
+      <c r="C69">
         <f>SUM(C17,C18,C19,C20,C12)</f>
         <v>13</v>
       </c>
-      <c r="D63">
-        <f t="shared" ref="D63:P63" si="9">SUM(D17,D18,D19,D20,D12)</f>
+      <c r="D69">
+        <f>SUM(D17,D18,D19,D20,D12)</f>
         <v>0.39</v>
       </c>
-      <c r="E63">
-        <f t="shared" si="9"/>
+      <c r="E69">
+        <f>SUM(E17,E18,E19,E20,E12)</f>
         <v>-13</v>
       </c>
-      <c r="F63">
-        <f t="shared" si="9"/>
+      <c r="F69">
+        <f>SUM(F17,F18,F19,F20,F12)</f>
         <v>-14</v>
       </c>
-      <c r="G63">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="H63">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="I63">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="J63">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="K63">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="L63">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="M63">
-        <f t="shared" si="9"/>
+      <c r="G69">
+        <f>SUM(G17,G18,G19,G20,G12)</f>
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <f>SUM(H17,H18,H19,H20,H12)</f>
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <f>SUM(I17,I18,I19,I20,I12)</f>
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <f>SUM(J17,J18,J19,J20,J12)</f>
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <f>SUM(K17,K18,K19,K20,K12)</f>
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <f>SUM(L17,L18,L19,L20,L12)</f>
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <f>SUM(M17,M18,M19,M20,M12)</f>
         <v>1500</v>
       </c>
-      <c r="N63">
-        <f t="shared" si="9"/>
+      <c r="N69">
+        <f>SUM(N17,N18,N19,N20,N12)</f>
         <v>24.000000000000004</v>
       </c>
-      <c r="O63">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="P63">
-        <f t="shared" si="9"/>
+      <c r="O69">
+        <f>SUM(O17,O18,O19,O20,O12)</f>
+        <v>0</v>
+      </c>
+      <c r="P69">
+        <f>SUM(P17,P18,P19,P20,P12)</f>
         <v>16.899999999999999</v>
       </c>
-      <c r="Q63">
-        <f t="shared" si="3"/>
+      <c r="Q69">
+        <f t="shared" si="1"/>
         <v>0.40559999999999996</v>
       </c>
-      <c r="S63" t="s">
+      <c r="S69" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="3" t="s">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C64">
+      <c r="C70">
         <f>SUM(C22,C21,C12,C19,C18,C17)</f>
         <v>17</v>
       </c>
-      <c r="D64">
-        <f t="shared" ref="D64:P64" si="10">SUM(D22,D21,D12,D19,D18,D17)</f>
+      <c r="D70">
+        <f>SUM(D22,D21,D12,D19,D18,D17)</f>
         <v>0.43</v>
       </c>
-      <c r="E64">
-        <f t="shared" si="10"/>
+      <c r="E70">
+        <f>SUM(E22,E21,E12,E19,E18,E17)</f>
         <v>-6</v>
       </c>
-      <c r="F64">
-        <f t="shared" si="10"/>
+      <c r="F70">
+        <f>SUM(F22,F21,F12,F19,F18,F17)</f>
         <v>-6</v>
       </c>
-      <c r="G64">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H64">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="I64">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="J64">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="K64">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="L64">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="M64">
-        <f t="shared" si="10"/>
+      <c r="G70">
+        <f>SUM(G22,G21,G12,G19,G18,G17)</f>
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <f>SUM(H22,H21,H12,H19,H18,H17)</f>
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <f>SUM(I22,I21,I12,I19,I18,I17)</f>
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <f>SUM(J22,J21,J12,J19,J18,J17)</f>
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <f>SUM(K22,K21,K12,K19,K18,K17)</f>
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <f>SUM(L22,L21,L12,L19,L18,L17)</f>
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <f>SUM(M22,M21,M12,M19,M18,M17)</f>
         <v>1850</v>
       </c>
-      <c r="N64">
-        <f t="shared" si="10"/>
+      <c r="N70">
+        <f>SUM(N22,N21,N12,N19,N18,N17)</f>
         <v>16.8</v>
       </c>
-      <c r="O64">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P64">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Q64">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q65">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5" t="s">
+      <c r="O70">
+        <f>SUM(O22,O21,O12,O19,O18,O17)</f>
+        <v>0</v>
+      </c>
+      <c r="P70">
+        <f>SUM(P22,P21,P12,P19,P18,P17)</f>
+        <v>0</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q71">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C66">
+      <c r="C72">
         <f>SUM(C23,C24,C25,C26)</f>
         <v>16</v>
       </c>
-      <c r="D66">
-        <f t="shared" ref="D66:P66" si="11">SUM(D23,D24,D25,D26)</f>
+      <c r="D72">
+        <f>SUM(D23,D24,D25,D26)</f>
         <v>0.35</v>
       </c>
-      <c r="E66">
-        <f t="shared" si="11"/>
+      <c r="E72">
+        <f>SUM(E23,E24,E25,E26)</f>
         <v>-11</v>
       </c>
-      <c r="F66">
-        <f t="shared" si="11"/>
+      <c r="F72">
+        <f>SUM(F23,F24,F25,F26)</f>
         <v>-11</v>
       </c>
-      <c r="G66">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="H66">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="I66">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="J66">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="K66">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="L66">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="M66">
-        <f t="shared" si="11"/>
+      <c r="G72">
+        <f>SUM(G23,G24,G25,G26)</f>
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <f>SUM(H23,H24,H25,H26)</f>
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <f>SUM(I23,I24,I25,I26)</f>
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <f>SUM(J23,J24,J25,J26)</f>
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <f>SUM(K23,K24,K25,K26)</f>
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <f>SUM(L23,L24,L25,L26)</f>
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <f>SUM(M23,M24,M25,M26)</f>
         <v>1300</v>
       </c>
-      <c r="N66">
-        <f t="shared" si="11"/>
+      <c r="N72">
+        <f>SUM(N23,N24,N25,N26)</f>
         <v>24.400000000000002</v>
       </c>
-      <c r="O66">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="P66">
-        <f t="shared" si="11"/>
+      <c r="O72">
+        <f>SUM(O23,O24,O25,O26)</f>
+        <v>0</v>
+      </c>
+      <c r="P72">
+        <f>SUM(P23,P24,P25,P26)</f>
         <v>15</v>
       </c>
-      <c r="Q66">
-        <f t="shared" si="3"/>
+      <c r="Q72">
+        <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="S66" t="s">
+      <c r="S72" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q67">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="6" t="s">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q73">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A74" s="6"/>
+      <c r="B74" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Q68">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="B69" s="1" t="s">
+      <c r="Q74">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A75" s="6"/>
+      <c r="B75" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C69">
+      <c r="C75">
         <f>SUM(C29,C28,C27)</f>
         <v>19</v>
       </c>
-      <c r="D69">
-        <f t="shared" ref="D69:P69" si="12">SUM(D29,D28,D27)</f>
+      <c r="D75">
+        <f>SUM(D29,D28,D27)</f>
         <v>0.36</v>
       </c>
-      <c r="E69">
-        <f t="shared" si="12"/>
+      <c r="E75">
+        <f>SUM(E29,E28,E27)</f>
         <v>-9</v>
       </c>
-      <c r="F69">
-        <f t="shared" si="12"/>
+      <c r="F75">
+        <f>SUM(F29,F28,F27)</f>
         <v>-6</v>
       </c>
-      <c r="G69">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="I69">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J69">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="K69">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="L69">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="M69">
-        <f t="shared" si="12"/>
+      <c r="G75">
+        <f>SUM(G29,G28,G27)</f>
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <f>SUM(H29,H28,H27)</f>
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <f>SUM(I29,I28,I27)</f>
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <f>SUM(J29,J28,J27)</f>
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <f>SUM(K29,K28,K27)</f>
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <f>SUM(L29,L28,L27)</f>
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <f>SUM(M29,M28,M27)</f>
         <v>2000</v>
       </c>
-      <c r="N69">
-        <f t="shared" si="12"/>
+      <c r="N75">
+        <f>SUM(N29,N28,N27)</f>
         <v>22.599999999999998</v>
       </c>
-      <c r="O69">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="P69">
-        <f t="shared" si="12"/>
+      <c r="O75">
+        <f>SUM(O29,O28,O27)</f>
+        <v>0</v>
+      </c>
+      <c r="P75">
+        <f>SUM(P29,P28,P27)</f>
         <v>16.7</v>
       </c>
-      <c r="Q69">
-        <f t="shared" si="3"/>
+      <c r="Q75">
+        <f t="shared" si="1"/>
         <v>0.40079999999999999</v>
       </c>
-      <c r="S69" t="s">
+      <c r="S75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="2" t="s">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A76" s="6"/>
+      <c r="B76" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C70">
+      <c r="C76">
         <f>SUM(C31,C30,C27,C29)</f>
         <v>20</v>
       </c>
-      <c r="D70">
-        <f t="shared" ref="D70:P70" si="13">SUM(D31,D30,D27,D29)</f>
+      <c r="D76">
+        <f>SUM(D31,D30,D27,D29)</f>
         <v>0.35</v>
       </c>
-      <c r="E70">
-        <f t="shared" si="13"/>
+      <c r="E76">
+        <f>SUM(E31,E30,E27,E29)</f>
         <v>-4</v>
       </c>
-      <c r="F70">
-        <f t="shared" si="13"/>
+      <c r="F76">
+        <f>SUM(F31,F30,F27,F29)</f>
         <v>-4</v>
       </c>
-      <c r="G70">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="H70">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="I70">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="J70">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="K70">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="L70">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="M70">
-        <f t="shared" si="13"/>
+      <c r="G76">
+        <f>SUM(G31,G30,G27,G29)</f>
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <f>SUM(H31,H30,H27,H29)</f>
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <f>SUM(I31,I30,I27,I29)</f>
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <f>SUM(J31,J30,J27,J29)</f>
+        <v>0</v>
+      </c>
+      <c r="K76">
+        <f>SUM(K31,K30,K27,K29)</f>
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <f>SUM(L31,L30,L27,L29)</f>
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <f>SUM(M31,M30,M27,M29)</f>
         <v>2000</v>
       </c>
-      <c r="N70">
-        <f t="shared" si="13"/>
+      <c r="N76">
+        <f>SUM(N31,N30,N27,N29)</f>
         <v>18.600000000000001</v>
       </c>
-      <c r="O70">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="P70">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="Q70">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q71">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7" t="s">
+      <c r="O76">
+        <f>SUM(O31,O30,O27,O29)</f>
+        <v>0</v>
+      </c>
+      <c r="P76">
+        <f>SUM(P31,P30,P27,P29)</f>
+        <v>0</v>
+      </c>
+      <c r="Q76">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q77">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A78" s="7"/>
+      <c r="B78" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="Q72">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
-      <c r="B73" s="1" t="s">
+      <c r="Q78">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A79" s="7"/>
+      <c r="B79" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C73">
+      <c r="C79">
         <f>C35+C32</f>
         <v>18</v>
       </c>
-      <c r="D73">
-        <f t="shared" ref="D73:P73" si="14">D35+D32</f>
+      <c r="D79">
+        <f>D35+D32</f>
         <v>0.36</v>
       </c>
-      <c r="E73">
-        <f t="shared" si="14"/>
+      <c r="E79">
+        <f>E35+E32</f>
         <v>-9</v>
       </c>
-      <c r="F73">
-        <f t="shared" si="14"/>
+      <c r="F79">
+        <f>F35+F32</f>
         <v>-8</v>
       </c>
-      <c r="G73">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="H73">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="I73">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="J73">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="K73">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="L73">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="M73">
-        <f t="shared" si="14"/>
+      <c r="G79">
+        <f>G35+G32</f>
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <f>H35+H32</f>
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <f>I35+I32</f>
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <f>J35+J32</f>
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <f>K35+K32</f>
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <f>L35+L32</f>
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <f>M35+M32</f>
         <v>1450</v>
       </c>
-      <c r="N73">
-        <f t="shared" si="14"/>
+      <c r="N79">
+        <f>N35+N32</f>
         <v>22.799999999999997</v>
       </c>
-      <c r="O73">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="P73">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="Q73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A74" s="7"/>
-      <c r="B74" s="2" t="s">
+      <c r="O79">
+        <f>O35+O32</f>
+        <v>0</v>
+      </c>
+      <c r="P79">
+        <f>P35+P32</f>
+        <v>0</v>
+      </c>
+      <c r="Q79">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A80" s="7"/>
+      <c r="B80" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C74">
+      <c r="C80">
         <f>C36+C32</f>
         <v>16</v>
       </c>
-      <c r="D74">
-        <f t="shared" ref="D74:P74" si="15">D36+D32</f>
+      <c r="D80">
+        <f>D36+D32</f>
         <v>0.35</v>
       </c>
-      <c r="E74">
-        <f t="shared" si="15"/>
+      <c r="E80">
+        <f>E36+E32</f>
         <v>-12</v>
       </c>
-      <c r="F74">
-        <f t="shared" si="15"/>
+      <c r="F80">
+        <f>F36+F32</f>
         <v>-7</v>
       </c>
-      <c r="G74">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="H74">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="I74">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="J74">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="K74">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="L74">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="M74">
-        <f t="shared" si="15"/>
+      <c r="G80">
+        <f>G36+G32</f>
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <f>H36+H32</f>
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <f>I36+I32</f>
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <f>J36+J32</f>
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <f>K36+K32</f>
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <f>L36+L32</f>
+        <v>0</v>
+      </c>
+      <c r="M80">
+        <f>M36+M32</f>
         <v>1500</v>
       </c>
-      <c r="N74">
-        <f t="shared" si="15"/>
+      <c r="N80">
+        <f>N36+N32</f>
         <v>22.8</v>
       </c>
-      <c r="O74">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="P74">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="Q74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
-      <c r="B75" s="1" t="s">
+      <c r="O80">
+        <f>O36+O32</f>
+        <v>0</v>
+      </c>
+      <c r="P80">
+        <f>P36+P32</f>
+        <v>0</v>
+      </c>
+      <c r="Q80">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A81" s="7"/>
+      <c r="B81" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A82" s="7"/>
+      <c r="B82" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C75">
+      <c r="C82">
         <f>SUM(C35,C34)</f>
         <v>17</v>
       </c>
-      <c r="D75">
-        <f t="shared" ref="D75:P75" si="16">SUM(D35,D34)</f>
-        <v>0.33</v>
-      </c>
-      <c r="E75">
-        <f t="shared" si="16"/>
+      <c r="D82">
+        <f>SUM(D35,D34)</f>
+        <v>0.34</v>
+      </c>
+      <c r="E82">
+        <f>SUM(E35,E34)</f>
         <v>-9</v>
       </c>
-      <c r="F75">
-        <f t="shared" si="16"/>
-        <v>-8</v>
-      </c>
-      <c r="G75">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="H75">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="I75">
-        <f t="shared" si="16"/>
-        <v>-0.1</v>
-      </c>
-      <c r="J75">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="K75">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="L75">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="M75">
-        <f t="shared" si="16"/>
+      <c r="F82">
+        <f>SUM(F35,F34)</f>
+        <v>-9</v>
+      </c>
+      <c r="G82">
+        <f>SUM(G35,G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <f>SUM(H35,H34)</f>
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <f>SUM(I35,I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <f>SUM(J35,J34)</f>
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <f>SUM(K35,K34)</f>
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <f>SUM(L35,L34)</f>
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <f>SUM(M35,M34)</f>
         <v>1200</v>
       </c>
-      <c r="N75">
-        <f t="shared" si="16"/>
-        <v>22.9</v>
-      </c>
-      <c r="O75">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="P75">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="Q75">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S75" t="s">
+      <c r="N82">
+        <f>SUM(N35,N34)</f>
+        <v>22.799999999999997</v>
+      </c>
+      <c r="O82">
+        <f>SUM(O35,O34)</f>
+        <v>0</v>
+      </c>
+      <c r="P82">
+        <f>SUM(P35,P34)</f>
+        <v>0</v>
+      </c>
+      <c r="Q82">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S82" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A76" s="7"/>
-      <c r="B76" s="2" t="s">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A83" s="7"/>
+      <c r="B83" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C76">
+      <c r="C83">
         <f>SUM(C36,C34)</f>
         <v>15</v>
       </c>
-      <c r="D76">
-        <f t="shared" ref="D76:P76" si="17">SUM(D36,D34)</f>
-        <v>0.32</v>
-      </c>
-      <c r="E76">
-        <f t="shared" si="17"/>
+      <c r="D83">
+        <f>SUM(D36,D34)</f>
+        <v>0.33</v>
+      </c>
+      <c r="E83">
+        <f>SUM(E36,E34)</f>
         <v>-12</v>
       </c>
-      <c r="F76">
-        <f t="shared" si="17"/>
-        <v>-7</v>
-      </c>
-      <c r="G76">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="H76">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="I76">
-        <f t="shared" si="17"/>
-        <v>-0.1</v>
-      </c>
-      <c r="J76">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="K76">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="L76">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="M76">
-        <f t="shared" si="17"/>
+      <c r="F83">
+        <f>SUM(F36,F34)</f>
+        <v>-8</v>
+      </c>
+      <c r="G83">
+        <f>SUM(G36,G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <f>SUM(H36,H34)</f>
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <f>SUM(I36,I34)</f>
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <f>SUM(J36,J34)</f>
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <f>SUM(K36,K34)</f>
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <f>SUM(L36,L34)</f>
+        <v>0</v>
+      </c>
+      <c r="M83">
+        <f>SUM(M36,M34)</f>
         <v>1250</v>
       </c>
-      <c r="N76">
+      <c r="N83">
         <f>SUM(N36,N34)</f>
-        <v>22.900000000000002</v>
-      </c>
-      <c r="O76">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="P76">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Q76">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S76" t="s">
+        <v>22.8</v>
+      </c>
+      <c r="O83">
+        <f>SUM(O36,O34)</f>
+        <v>0</v>
+      </c>
+      <c r="P83">
+        <f>SUM(P36,P34)</f>
+        <v>0</v>
+      </c>
+      <c r="Q83">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S83" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q77">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A78" s="8"/>
-      <c r="B78" s="8" t="s">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q84">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A85" s="8"/>
+      <c r="B85" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C78">
+      <c r="C85">
         <f>SUM(C37,C38)</f>
         <v>18</v>
       </c>
-      <c r="D78">
+      <c r="D85">
         <f>SUM(D37,D38)</f>
         <v>0.28999999999999998</v>
       </c>
-      <c r="E78">
+      <c r="E85">
         <f>SUM(E37,E38)</f>
         <v>-9</v>
       </c>
-      <c r="F78">
+      <c r="F85">
         <f>SUM(F37,F38)</f>
         <v>-8</v>
       </c>
-      <c r="M78">
+      <c r="G85">
+        <f>SUM(G37,G38)</f>
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <f>SUM(H37,H38)</f>
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <f>SUM(I37,I38)</f>
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <f>SUM(J37,J38)</f>
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <f>SUM(K37,K38)</f>
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <f>SUM(L37,L38)</f>
+        <v>0</v>
+      </c>
+      <c r="M85">
         <f>SUM(M37,M38)</f>
         <v>1200</v>
       </c>
-      <c r="N78">
+      <c r="N85">
         <f>SUM(N37,N38)</f>
         <v>24.2</v>
       </c>
-      <c r="P78">
+      <c r="O85">
+        <f>SUM(O37,O38)</f>
+        <v>0</v>
+      </c>
+      <c r="P85">
         <f>SUM(P37,P38)</f>
         <v>12.5</v>
       </c>
-      <c r="Q78">
-        <f t="shared" si="3"/>
+      <c r="Q85">
+        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="S78" t="s">
+      <c r="S85" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q79">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A80" s="10"/>
-      <c r="B80" s="10" t="s">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q86">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A87" s="10"/>
+      <c r="B87" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C80">
+      <c r="C87">
         <f>SUM(C39,C40)</f>
         <v>14</v>
       </c>
-      <c r="D80">
+      <c r="D87">
         <f>SUM(D39,D40)</f>
         <v>0.3</v>
       </c>
-      <c r="E80">
+      <c r="E87">
         <f>SUM(E39,E40)</f>
         <v>-11</v>
       </c>
-      <c r="F80">
+      <c r="F87">
         <f>SUM(F39,F40)</f>
         <v>-11</v>
       </c>
-      <c r="M80">
+      <c r="G87">
+        <f>SUM(G39,G40)</f>
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <f>SUM(H39,H40)</f>
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <f>SUM(I39,I40)</f>
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <f>SUM(J39,J40)</f>
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <f>SUM(K39,K40)</f>
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <f>SUM(L39,L40)</f>
+        <v>0</v>
+      </c>
+      <c r="M87">
         <f>SUM(M39,M40)</f>
         <v>1350</v>
       </c>
-      <c r="N80">
+      <c r="N87">
         <f>SUM(N39,N40)</f>
         <v>23.400000000000002</v>
       </c>
-      <c r="P80">
+      <c r="O87">
+        <f>SUM(O39,O40)</f>
+        <v>0</v>
+      </c>
+      <c r="P87">
         <f>SUM(P39,P40)</f>
         <v>15</v>
       </c>
-      <c r="Q80">
-        <f t="shared" si="3"/>
+      <c r="Q87">
+        <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
-      <c r="S80" t="s">
+      <c r="S87" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A81" s="10"/>
-      <c r="B81" s="10" t="s">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A88" s="10"/>
+      <c r="B88" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C81">
+      <c r="C88">
         <f>C39</f>
         <v>13</v>
       </c>
-      <c r="D81">
-        <f>D39</f>
+      <c r="D88">
+        <f t="shared" ref="D88:P88" si="2">D39</f>
         <v>0.21</v>
       </c>
-      <c r="E81">
-        <f>E39</f>
+      <c r="E88">
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
-      <c r="F81">
-        <f>F39</f>
+      <c r="F88">
+        <f t="shared" si="2"/>
         <v>-10</v>
       </c>
-      <c r="M81">
-        <f>M39</f>
+      <c r="G88">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M88">
+        <f t="shared" si="2"/>
         <v>750</v>
       </c>
-      <c r="N81">
-        <f>N39</f>
+      <c r="N88">
+        <f t="shared" si="2"/>
         <v>22.8</v>
       </c>
-      <c r="P81">
+      <c r="O88">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P88">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="Q81">
-        <f t="shared" si="3"/>
+      <c r="Q88">
+        <f t="shared" si="1"/>
         <v>0.216</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q82">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4" t="s">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q89">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+      <c r="B90" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C83">
+      <c r="C90">
         <f>C41</f>
         <v>16</v>
       </c>
-      <c r="D83">
-        <f>D41</f>
+      <c r="D90">
+        <f t="shared" ref="D90:P90" si="3">D41</f>
         <v>0.33</v>
       </c>
-      <c r="E83">
-        <f>E41</f>
+      <c r="E90">
+        <f t="shared" si="3"/>
         <v>-7</v>
       </c>
-      <c r="F83">
-        <f>F41</f>
+      <c r="F90">
+        <f t="shared" si="3"/>
         <v>-14</v>
       </c>
-      <c r="M83">
-        <f>M41</f>
+      <c r="G90">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K90">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L90">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M90">
+        <f t="shared" si="3"/>
         <v>700</v>
       </c>
-      <c r="N83">
-        <f>N41</f>
+      <c r="N90">
+        <f t="shared" si="3"/>
         <v>23.4</v>
       </c>
-      <c r="P83">
-        <f>P41</f>
+      <c r="O90">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P90">
+        <f t="shared" si="3"/>
         <v>14.4</v>
       </c>
-      <c r="Q83">
-        <f t="shared" si="3"/>
+      <c r="Q90">
+        <f t="shared" si="1"/>
         <v>0.34560000000000002</v>
       </c>
-      <c r="S83" t="s">
+      <c r="S90" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q84">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
-      <c r="B85" s="11" t="s">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q91">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A92" s="13"/>
+      <c r="B92" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C92">
+        <f>C42+C43</f>
+        <v>11</v>
+      </c>
+      <c r="D92">
+        <f t="shared" ref="D92:P92" si="4">D42+D43</f>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="4"/>
+        <v>-16</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="4"/>
+        <v>-21</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J92">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M92">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+      <c r="N92">
+        <f t="shared" si="4"/>
+        <v>27.400000000000002</v>
+      </c>
+      <c r="O92">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P92">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="Q92">
+        <f t="shared" si="1"/>
+        <v>0.45600000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q93">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A94" s="9"/>
+      <c r="B94" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q94">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A95" s="9"/>
+      <c r="B95" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C95">
+        <f>C47+C48</f>
+        <v>18</v>
+      </c>
+      <c r="D95">
+        <f>D47+D48</f>
+        <v>0.26</v>
+      </c>
+      <c r="E95">
+        <f>E47+E48</f>
+        <v>-11</v>
+      </c>
+      <c r="F95">
+        <f>F47+F48</f>
+        <v>-6</v>
+      </c>
+      <c r="G95">
+        <f>G47+G48</f>
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <f>H47+H48</f>
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <f>I47+I48</f>
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <f>J47+J48</f>
+        <v>0</v>
+      </c>
+      <c r="K95">
+        <f>K47+K48</f>
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <f>L47+L48</f>
+        <v>0</v>
+      </c>
+      <c r="M95">
+        <f>M47+M48</f>
+        <v>600</v>
+      </c>
+      <c r="N95">
+        <f>N47+N48</f>
+        <v>25.2</v>
+      </c>
+      <c r="O95">
+        <f>O47+O48</f>
+        <v>0</v>
+      </c>
+      <c r="P95">
+        <f>P47+P48</f>
+        <v>0</v>
+      </c>
+      <c r="Q95">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A96" s="9"/>
+      <c r="B96" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C96">
+        <f>C47+C49</f>
+        <v>20</v>
+      </c>
+      <c r="D96">
+        <f>D47+D49</f>
+        <v>0.26</v>
+      </c>
+      <c r="E96">
+        <f>E47+E49</f>
+        <v>-10</v>
+      </c>
+      <c r="F96">
+        <f>F47+F49</f>
+        <v>-4</v>
+      </c>
+      <c r="G96">
+        <f>G47+G49</f>
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <f>H47+H49</f>
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <f>I47+I49</f>
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <f>J47+J49</f>
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <f>K47+K49</f>
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <f>L47+L49</f>
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <f>M47+M49</f>
+        <v>600</v>
+      </c>
+      <c r="N96">
+        <f>N47+N49</f>
+        <v>25.2</v>
+      </c>
+      <c r="O96">
+        <f>O47+O49</f>
+        <v>0</v>
+      </c>
+      <c r="P96">
+        <f>P47+P49</f>
+        <v>0</v>
+      </c>
+      <c r="Q96">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q97">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98" s="17"/>
+      <c r="B98" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q98">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99" s="17"/>
+      <c r="B99" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C99">
+        <f>C50+C51</f>
+        <v>10</v>
+      </c>
+      <c r="D99">
+        <f>D50+D51</f>
+        <v>0.32</v>
+      </c>
+      <c r="E99">
+        <f>E50+E51</f>
+        <v>-14</v>
+      </c>
+      <c r="F99">
+        <f>F50+F51</f>
+        <v>-17</v>
+      </c>
+      <c r="G99">
+        <f>G50+G51</f>
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <f>H50+H51</f>
+        <v>0.05</v>
+      </c>
+      <c r="I99">
+        <f>I50+I51</f>
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <f>J50+J51</f>
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <f>K50+K51</f>
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <f>L50+L51</f>
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <f>M50+M51</f>
+        <v>2000</v>
+      </c>
+      <c r="N99">
+        <f>N50+N51</f>
+        <v>25</v>
+      </c>
+      <c r="O99">
+        <f>O50+O51</f>
+        <v>0</v>
+      </c>
+      <c r="P99">
+        <f>P50+P51</f>
+        <v>0</v>
+      </c>
+      <c r="Q99">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100" s="17"/>
+      <c r="B100" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C100">
+        <f>C50+C52</f>
+        <v>12</v>
+      </c>
+      <c r="D100">
+        <f>D50+D52</f>
+        <v>0.32</v>
+      </c>
+      <c r="E100">
+        <f>E50+E52</f>
+        <v>-13</v>
+      </c>
+      <c r="F100">
+        <f>F50+F52</f>
+        <v>-15</v>
+      </c>
+      <c r="G100">
+        <f>G50+G52</f>
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <f>H50+H52</f>
+        <v>0.05</v>
+      </c>
+      <c r="I100">
+        <f>I50+I52</f>
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <f>J50+J52</f>
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <f>K50+K52</f>
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <f>L50+L52</f>
+        <v>0</v>
+      </c>
+      <c r="M100">
+        <f>M50+M52</f>
+        <v>2000</v>
+      </c>
+      <c r="N100">
+        <f>N50+N52</f>
+        <v>25</v>
+      </c>
+      <c r="O100">
+        <f>O50+O52</f>
+        <v>0</v>
+      </c>
+      <c r="P100">
+        <f>P50+P52</f>
+        <v>0</v>
+      </c>
+      <c r="Q100">
+        <f>P100*0.024</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101" s="18"/>
+      <c r="B101" s="18"/>
+      <c r="Q101">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102" s="11"/>
+      <c r="B102" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="Q85">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A86" s="11"/>
-      <c r="B86" s="12" t="s">
+      <c r="Q102">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103" s="11"/>
+      <c r="B103" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C86">
-        <f>SUM(C50,C47)</f>
+      <c r="C103">
+        <f>SUM(C56,C53)</f>
         <v>17</v>
       </c>
-      <c r="D86">
-        <f>SUM(D50,D47)</f>
+      <c r="D103">
+        <f>SUM(D56,D53)</f>
         <v>0.44000000000000006</v>
       </c>
-      <c r="E86">
-        <f>SUM(E50,E47)</f>
+      <c r="E103">
+        <f>SUM(E56,E53)</f>
         <v>-11</v>
       </c>
-      <c r="F86">
-        <f>SUM(F50,F47)</f>
+      <c r="F103">
+        <f>SUM(F56,F53)</f>
         <v>-10</v>
       </c>
-      <c r="M86">
-        <f>SUM(M50,M47)</f>
+      <c r="G103">
+        <f>SUM(G56,G53)</f>
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <f>SUM(H56,H53)</f>
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <f>SUM(I56,I53)</f>
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <f>SUM(J56,J53)</f>
+        <v>0</v>
+      </c>
+      <c r="K103">
+        <f>SUM(K56,K53)</f>
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <f>SUM(L56,L53)</f>
+        <v>0</v>
+      </c>
+      <c r="M103">
+        <f>SUM(M56,M53)</f>
         <v>2600</v>
       </c>
-      <c r="N86">
-        <f>SUM(N50,N47)</f>
+      <c r="N103">
+        <f>SUM(N56,N53)</f>
         <v>23</v>
       </c>
-      <c r="P86">
-        <f>SUM(P50,P47)</f>
+      <c r="O103">
+        <f>SUM(O56,O53)</f>
+        <v>0</v>
+      </c>
+      <c r="P103">
+        <f>SUM(P56,P53)</f>
         <v>22.4</v>
       </c>
-      <c r="Q86">
-        <f t="shared" si="3"/>
+      <c r="Q103">
+        <f t="shared" si="1"/>
         <v>0.53759999999999997</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q87">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A88" s="11"/>
-      <c r="B88" s="11" t="s">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q104">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A105" s="11"/>
+      <c r="B105" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="Q88">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A89" s="11"/>
-      <c r="B89" s="12" t="s">
+      <c r="Q105">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A106" s="11"/>
+      <c r="B106" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C89">
-        <f>SUM(C50,C48)</f>
+      <c r="C106">
+        <f>SUM(C56,C54)</f>
         <v>17</v>
       </c>
-      <c r="D89">
-        <f>SUM(D50,D48)</f>
+      <c r="D106">
+        <f>SUM(D56,D54)</f>
         <v>0.47000000000000003</v>
       </c>
-      <c r="E89">
-        <f>SUM(E50,E48)</f>
+      <c r="E106">
+        <f>SUM(E56,E54)</f>
         <v>-11</v>
       </c>
-      <c r="F89">
-        <f>SUM(F50,F48)</f>
+      <c r="F106">
+        <f>SUM(F56,F54)</f>
         <v>-10</v>
       </c>
-      <c r="M89">
-        <f>SUM(M50,M48)</f>
+      <c r="G106">
+        <f>SUM(G56,G54)</f>
+        <v>0</v>
+      </c>
+      <c r="H106">
+        <f>SUM(H56,H54)</f>
+        <v>0</v>
+      </c>
+      <c r="I106">
+        <f>SUM(I56,I54)</f>
+        <v>0</v>
+      </c>
+      <c r="J106">
+        <f>SUM(J56,J54)</f>
+        <v>0</v>
+      </c>
+      <c r="K106">
+        <f>SUM(K56,K54)</f>
+        <v>0</v>
+      </c>
+      <c r="L106">
+        <f>SUM(L56,L54)</f>
+        <v>0</v>
+      </c>
+      <c r="M106">
+        <f>SUM(M56,M54)</f>
         <v>1800</v>
       </c>
-      <c r="N89">
-        <f>SUM(N50,N48)</f>
+      <c r="N106">
+        <f>SUM(N56,N54)</f>
         <v>22.4</v>
       </c>
-      <c r="P89">
-        <f>SUM(P50,P48)</f>
+      <c r="O106">
+        <f>SUM(O56,O54)</f>
+        <v>0</v>
+      </c>
+      <c r="P106">
+        <f>SUM(P56,P54)</f>
         <v>24.75</v>
       </c>
-      <c r="Q89">
-        <f t="shared" si="3"/>
+      <c r="Q106">
+        <f t="shared" si="1"/>
         <v>0.59399999999999997</v>
       </c>
     </row>

</xml_diff>